<commit_message>
adding cmpd search, some tests and documentation
</commit_message>
<xml_diff>
--- a/tests/test_acasclient/1_1_Generic.xlsx
+++ b/tests/test_acasclient/1_1_Generic.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbolt/Documents/mcneilco/oss/acasclient/tests/test_acasclient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B138285-2D15-F34A-98CD-BFDC28E23747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE50372E-057B-324A-99FE-B73329299ABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="20220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>

</xml_diff>